<commit_message>
ีupdate data part 2
</commit_message>
<xml_diff>
--- a/process_data/info_cluster2.xlsx
+++ b/process_data/info_cluster2.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pantc\Documents\final_stat_pant\process_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8604E0-39E1-41A9-B6F5-62D577B9CB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-21720" yWindow="645" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Agriculture, forestry and fishing</t>
   </si>
@@ -80,13 +87,16 @@
   </si>
   <si>
     <t>cluster_id</t>
+  </si>
+  <si>
+    <t>Cluster ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,17 +148,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -195,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +246,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,6 +298,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,14 +491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="A1:G23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -463,15 +520,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>39635.03780546667</v>
+        <v>39635.037805466673</v>
       </c>
       <c r="C2">
-        <v>2497.921177666667</v>
+        <v>2497.9211776666671</v>
       </c>
       <c r="D2">
         <v>14268.93262138182</v>
@@ -480,87 +537,87 @@
         <v>11630.2204158</v>
       </c>
       <c r="F2">
-        <v>19900.41089966667</v>
+        <v>19900.410899666669</v>
       </c>
       <c r="G2">
-        <v>13480.67156139091</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>13480.671561390909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4715.167163033333</v>
+        <v>4715.1671630333331</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1218.763802109091</v>
+        <v>1218.7638021090911</v>
       </c>
       <c r="E3">
-        <v>2506.066275933334</v>
+        <v>2506.0662759333341</v>
       </c>
       <c r="F3">
-        <v>262056.5167253333</v>
+        <v>262056.51672533329</v>
       </c>
       <c r="G3">
         <v>1209.732278309091</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>34002.49958466668</v>
+        <v>34002.499584666679</v>
       </c>
       <c r="C4">
-        <v>606117.460113</v>
+        <v>606117.46011300001</v>
       </c>
       <c r="D4">
-        <v>9505.12059256364</v>
+        <v>9505.1205925636405</v>
       </c>
       <c r="E4">
         <v>227791.1941861333</v>
       </c>
       <c r="F4">
-        <v>450453.8644803333</v>
+        <v>450453.86448033329</v>
       </c>
       <c r="G4">
-        <v>8906.611113645455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>8906.6111136454547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6694.721087799999</v>
+        <v>6694.7210877999987</v>
       </c>
       <c r="C5">
-        <v>37794.57709233333</v>
+        <v>37794.577092333333</v>
       </c>
       <c r="D5">
-        <v>947.572874436364</v>
+        <v>947.57287443636403</v>
       </c>
       <c r="E5">
-        <v>16692.9664857</v>
+        <v>16692.966485699999</v>
       </c>
       <c r="F5">
-        <v>71150.62374366667</v>
+        <v>71150.623743666671</v>
       </c>
       <c r="G5">
         <v>1011.772839554545</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>587.2097215666668</v>
+        <v>587.20972156666676</v>
       </c>
       <c r="C6">
         <v>23224.49829066667</v>
@@ -575,125 +632,125 @@
         <v>2455.625102</v>
       </c>
       <c r="G6">
-        <v>204.7707966727272</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>204.77079667272719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>7085.726371533331</v>
+        <v>7085.7263715333311</v>
       </c>
       <c r="C7">
-        <v>108017.5609026667</v>
+        <v>108017.56090266669</v>
       </c>
       <c r="D7">
-        <v>2459.166580836363</v>
+        <v>2459.1665808363632</v>
       </c>
       <c r="E7">
-        <v>8769.826678533334</v>
+        <v>8769.8266785333344</v>
       </c>
       <c r="F7">
-        <v>7359.746358666666</v>
+        <v>7359.7463586666663</v>
       </c>
       <c r="G7">
-        <v>2264.131521072727</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>2264.1315210727271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>23948.2290301</v>
+        <v>23948.229030099999</v>
       </c>
       <c r="C8">
-        <v>1115444.685529333</v>
+        <v>1115444.6855293331</v>
       </c>
       <c r="D8">
         <v>7832.158000090908</v>
       </c>
       <c r="E8">
-        <v>56122.03586826666</v>
+        <v>56122.035868266663</v>
       </c>
       <c r="F8">
-        <v>74112.53675166667</v>
+        <v>74112.536751666674</v>
       </c>
       <c r="G8">
-        <v>6962.981849863636</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>6962.9818498636359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6525.747901300001</v>
+        <v>6525.7479013000011</v>
       </c>
       <c r="C9">
-        <v>381749.605188</v>
+        <v>381749.60518800002</v>
       </c>
       <c r="D9">
-        <v>2736.576858218183</v>
+        <v>2736.5768582181831</v>
       </c>
       <c r="E9">
-        <v>30517.72949366666</v>
+        <v>30517.729493666659</v>
       </c>
       <c r="F9">
-        <v>19894.52735866666</v>
+        <v>19894.527358666659</v>
       </c>
       <c r="G9">
         <v>2464.419487000001</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8458.607645200002</v>
+        <v>8458.6076452000016</v>
       </c>
       <c r="C10">
-        <v>441702.061184</v>
+        <v>441702.06118399999</v>
       </c>
       <c r="D10">
-        <v>3777.716303</v>
+        <v>3777.7163030000002</v>
       </c>
       <c r="E10">
-        <v>9797.588491100001</v>
+        <v>9797.5884911000012</v>
       </c>
       <c r="F10">
-        <v>3655.038678333333</v>
+        <v>3655.0386783333329</v>
       </c>
       <c r="G10">
-        <v>3108.971905009091</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>3108.9719050090912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1553.0625142</v>
+        <v>1553.0625141999999</v>
       </c>
       <c r="C11">
-        <v>275821.5433836667</v>
+        <v>275821.54338366672</v>
       </c>
       <c r="D11">
-        <v>516.0165885454546</v>
+        <v>516.01658854545462</v>
       </c>
       <c r="E11">
-        <v>4407.836327133334</v>
+        <v>4407.8363271333337</v>
       </c>
       <c r="F11">
         <v>1540.530229333333</v>
       </c>
       <c r="G11">
-        <v>425.5854425454546</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>425.58544254545461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,7 +758,7 @@
         <v>10195.26597843333</v>
       </c>
       <c r="C12">
-        <v>713617.4343966668</v>
+        <v>713617.43439666682</v>
       </c>
       <c r="D12">
         <v>3988.515720599999</v>
@@ -713,102 +770,102 @@
         <v>11462.769059</v>
       </c>
       <c r="G12">
-        <v>3693.754699663636</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>3693.7546996636361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5626.7940507</v>
+        <v>5626.7940507000003</v>
       </c>
       <c r="C13">
         <v>100784.5932633333</v>
       </c>
       <c r="D13">
-        <v>2478.417473981818</v>
+        <v>2478.4174739818181</v>
       </c>
       <c r="E13">
-        <v>8610.291251166665</v>
+        <v>8610.2912511666655</v>
       </c>
       <c r="F13">
         <v>5934.708247333333</v>
       </c>
       <c r="G13">
-        <v>2264.872358263636</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>2264.8723582636362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>329.1330822333334</v>
+        <v>329.13308223333343</v>
       </c>
       <c r="C14">
         <v>212400.4519626667</v>
       </c>
       <c r="D14">
-        <v>56.59986470909092</v>
+        <v>56.599864709090923</v>
       </c>
       <c r="E14">
-        <v>2825.256865966667</v>
+        <v>2825.2568659666672</v>
       </c>
       <c r="F14">
-        <v>25262.198098</v>
+        <v>25262.198098000001</v>
       </c>
       <c r="G14">
-        <v>49.03138834545455</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>49.031388345454552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1283.271308433333</v>
+        <v>1283.2713084333329</v>
       </c>
       <c r="C15">
-        <v>148614.5310706666</v>
+        <v>148614.53107066659</v>
       </c>
       <c r="D15">
-        <v>574.6822212545454</v>
+        <v>574.68222125454542</v>
       </c>
       <c r="E15">
-        <v>5619.870398866668</v>
+        <v>5619.8703988666684</v>
       </c>
       <c r="F15">
-        <v>4502.965577999999</v>
+        <v>4502.9655779999994</v>
       </c>
       <c r="G15">
-        <v>505.2345450454544</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>505.23454504545441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>8932.369923099999</v>
+        <v>8932.3699230999991</v>
       </c>
       <c r="C16">
-        <v>520194.3247333334</v>
+        <v>520194.32473333337</v>
       </c>
       <c r="D16">
-        <v>3641.912462636363</v>
+        <v>3641.9124626363632</v>
       </c>
       <c r="E16">
         <v>11137.20507086667</v>
       </c>
       <c r="F16">
-        <v>8253.248928999999</v>
+        <v>8253.2489289999994</v>
       </c>
       <c r="G16">
-        <v>3343.752528300002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>3343.7525283000018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -816,30 +873,30 @@
         <v>13029.35372166667</v>
       </c>
       <c r="C17">
-        <v>89610.24562666666</v>
+        <v>89610.245626666656</v>
       </c>
       <c r="D17">
         <v>6017.758319272727</v>
       </c>
       <c r="E17">
-        <v>8171.399804999999</v>
+        <v>8171.3998049999991</v>
       </c>
       <c r="F17">
         <v>3617.235470333334</v>
       </c>
       <c r="G17">
-        <v>5882.891307809091</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>5882.8913078090909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>5400.668005533333</v>
+        <v>5400.6680055333327</v>
       </c>
       <c r="C18">
-        <v>84743.54881633334</v>
+        <v>84743.548816333336</v>
       </c>
       <c r="D18">
         <v>2018.244600436364</v>
@@ -848,13 +905,13 @@
         <v>8270.376866333334</v>
       </c>
       <c r="F18">
-        <v>3173.940166666667</v>
+        <v>3173.9401666666672</v>
       </c>
       <c r="G18">
-        <v>1773.390828118182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>1773.3908281181821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -868,16 +925,16 @@
         <v>204.5653086181818</v>
       </c>
       <c r="E19">
-        <v>1815.4172883</v>
+        <v>1815.4172883000001</v>
       </c>
       <c r="F19">
-        <v>403.5010513333334</v>
+        <v>403.50105133333341</v>
       </c>
       <c r="G19">
         <v>165.8635095909091</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -891,50 +948,50 @@
         <v>605.9899240181818</v>
       </c>
       <c r="E20">
-        <v>4257.723959166667</v>
+        <v>4257.7239591666666</v>
       </c>
       <c r="F20">
-        <v>2228.824503333333</v>
+        <v>2228.8245033333328</v>
       </c>
       <c r="G20">
-        <v>569.2428068181817</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>569.24280681818175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>69195906.76666667</v>
+        <v>69195906.766666666</v>
       </c>
       <c r="C21">
-        <v>69203194.66666667</v>
+        <v>69203194.666666672</v>
       </c>
       <c r="D21">
         <v>69428454</v>
       </c>
       <c r="E21">
-        <v>69218432.7</v>
+        <v>69218432.700000003</v>
       </c>
       <c r="F21">
-        <v>69203194.66666667</v>
+        <v>69203194.666666672</v>
       </c>
       <c r="G21">
-        <v>69088396.78181818</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>69088396.781818181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>152463.4410666667</v>
+        <v>152463.44106666671</v>
       </c>
       <c r="C22">
-        <v>573019.2930000001</v>
+        <v>573019.29300000006</v>
       </c>
       <c r="D22">
-        <v>109676.7930727273</v>
+        <v>109676.79307272731</v>
       </c>
       <c r="E22">
         <v>361709.7166333333</v>
@@ -943,10 +1000,10 @@
         <v>1026253.370333333</v>
       </c>
       <c r="G22">
-        <v>102260.6309272727</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>102260.63092727269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -972,4 +1029,529 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88988759-DD82-4564-A71D-D74AE4B74853}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="71.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>39635.037805466673</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2497.9211776666671</v>
+      </c>
+      <c r="D2" s="2">
+        <v>14268.93262138182</v>
+      </c>
+      <c r="E2" s="2">
+        <v>11630.2204158</v>
+      </c>
+      <c r="F2" s="2">
+        <v>19900.410899666669</v>
+      </c>
+      <c r="G2" s="2">
+        <v>13480.671561390909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4715.1671630333331</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1218.7638021090911</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2506.0662759333341</v>
+      </c>
+      <c r="F3" s="2">
+        <v>262056.51672533329</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1209.732278309091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>34002.499584666701</v>
+      </c>
+      <c r="C4" s="2">
+        <v>606117.46011300001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9505.1205925636405</v>
+      </c>
+      <c r="E4" s="2">
+        <v>227791.1941861333</v>
+      </c>
+      <c r="F4" s="2">
+        <v>450453.86448033329</v>
+      </c>
+      <c r="G4" s="2">
+        <v>8906.6111136454547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6694.7210877999987</v>
+      </c>
+      <c r="C5" s="2">
+        <v>37794.577092333333</v>
+      </c>
+      <c r="D5" s="2">
+        <v>947.57287443636403</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16692.966485699999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>71150.623743666671</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1011.772839554545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>587.20972156666676</v>
+      </c>
+      <c r="C6" s="2">
+        <v>23224.49829066667</v>
+      </c>
+      <c r="D6" s="2">
+        <v>238.4606553636365</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2008.1917899</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2455.625102</v>
+      </c>
+      <c r="G6" s="2">
+        <v>204.77079667272719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7085.7263715333311</v>
+      </c>
+      <c r="C7" s="2">
+        <v>108017.56090266669</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2459.1665808363632</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8769.8266785333344</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7359.7463586666663</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2264.1315210727271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>23948.229030099999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1115444.6855293331</v>
+      </c>
+      <c r="D8" s="2">
+        <v>7832.158000090908</v>
+      </c>
+      <c r="E8" s="2">
+        <v>56122.035868266663</v>
+      </c>
+      <c r="F8" s="2">
+        <v>74112.536751666674</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6962.9818498636359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6525.7479013000011</v>
+      </c>
+      <c r="C9" s="2">
+        <v>381749.60518800002</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2736.5768582181831</v>
+      </c>
+      <c r="E9" s="2">
+        <v>30517.729493666659</v>
+      </c>
+      <c r="F9" s="2">
+        <v>19894.527358666659</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2464.419487000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8458.6076452000016</v>
+      </c>
+      <c r="C10" s="2">
+        <v>441702.06118399999</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3777.7163030000002</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9797.5884911000012</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3655.0386783333329</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3108.9719050090912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1553.0625141999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>275821.54338366672</v>
+      </c>
+      <c r="D11" s="2">
+        <v>516.01658854545462</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4407.8363271333337</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1540.530229333333</v>
+      </c>
+      <c r="G11" s="2">
+        <v>425.58544254545461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10195.26597843333</v>
+      </c>
+      <c r="C12" s="2">
+        <v>713617.43439666682</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3988.515720599999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>14226.05774453334</v>
+      </c>
+      <c r="F12" s="2">
+        <v>11462.769059</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3693.7546996636361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5626.7940507000003</v>
+      </c>
+      <c r="C13" s="2">
+        <v>100784.5932633333</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2478.4174739818181</v>
+      </c>
+      <c r="E13" s="2">
+        <v>8610.2912511666655</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5934.708247333333</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2264.8723582636362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>329.13308223333343</v>
+      </c>
+      <c r="C14" s="2">
+        <v>212400.4519626667</v>
+      </c>
+      <c r="D14" s="2">
+        <v>56.599864709090923</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2825.2568659666672</v>
+      </c>
+      <c r="F14" s="2">
+        <v>25262.198098000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>49.031388345454552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1283.2713084333329</v>
+      </c>
+      <c r="C15" s="2">
+        <v>148614.53107066659</v>
+      </c>
+      <c r="D15" s="2">
+        <v>574.68222125454542</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5619.8703988666684</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4502.9655779999994</v>
+      </c>
+      <c r="G15" s="2">
+        <v>505.23454504545441</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8932.3699230999991</v>
+      </c>
+      <c r="C16" s="2">
+        <v>520194.32473333337</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3641.9124626363632</v>
+      </c>
+      <c r="E16" s="2">
+        <v>11137.20507086667</v>
+      </c>
+      <c r="F16" s="2">
+        <v>8253.2489289999994</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3343.7525283000018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13029.35372166667</v>
+      </c>
+      <c r="C17" s="2">
+        <v>89610.245626666656</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6017.758319272727</v>
+      </c>
+      <c r="E17" s="2">
+        <v>8171.3998049999991</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3617.235470333334</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5882.8913078090909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5400.6680055333327</v>
+      </c>
+      <c r="C18" s="2">
+        <v>84743.548816333336</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2018.244600436364</v>
+      </c>
+      <c r="E18" s="2">
+        <v>8270.376866333334</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3173.9401666666672</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1773.3908281181821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>354.8710049</v>
+      </c>
+      <c r="C19" s="2">
+        <v>59605.905046</v>
+      </c>
+      <c r="D19" s="2">
+        <v>204.5653086181818</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1815.4172883000001</v>
+      </c>
+      <c r="F19" s="2">
+        <v>403.50105133333341</v>
+      </c>
+      <c r="G19" s="2">
+        <v>165.8635095909091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1474.998930266667</v>
+      </c>
+      <c r="C20" s="2">
+        <v>140995.2456496667</v>
+      </c>
+      <c r="D20" s="2">
+        <v>605.9899240181818</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4257.7239591666666</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2228.8245033333328</v>
+      </c>
+      <c r="G20" s="2">
+        <v>569.24280681818175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>69195906.766666666</v>
+      </c>
+      <c r="C21" s="2">
+        <v>69203194.666666672</v>
+      </c>
+      <c r="D21" s="2">
+        <v>69428454</v>
+      </c>
+      <c r="E21" s="2">
+        <v>69218432.700000003</v>
+      </c>
+      <c r="F21" s="2">
+        <v>69203194.666666672</v>
+      </c>
+      <c r="G21" s="2">
+        <v>69088396.781818181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
+        <v>152463.44106666671</v>
+      </c>
+      <c r="C22" s="2">
+        <v>573019.29300000006</v>
+      </c>
+      <c r="D22" s="2">
+        <v>109676.79307272731</v>
+      </c>
+      <c r="E22" s="2">
+        <v>361709.7166333333</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1026253.370333333</v>
+      </c>
+      <c r="G22" s="2">
+        <v>102260.63092727269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>